<commit_message>
Adding new points to the sounding excel sheet
</commit_message>
<xml_diff>
--- a/Sounding_calculation.xlsx
+++ b/Sounding_calculation.xlsx
@@ -8,14 +8,41 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/FireFlux_med/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D51B1CDD-FB0C-BD45-B255-C8447F02C708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B383A-D337-154E-9C92-E97D98C8343D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{BE37ABCF-635B-BF46-BE11-3CD29516FACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$B$26</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_lin" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$G$18</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">3</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">2</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
   <si>
     <t>Original input_Sounding</t>
   </si>
@@ -95,6 +122,15 @@
   </si>
   <si>
     <t>actual ws</t>
+  </si>
+  <si>
+    <t>These are unrealistic</t>
+  </si>
+  <si>
+    <t>thoughts</t>
+  </si>
+  <si>
+    <t>f</t>
   </si>
 </sst>
 </file>
@@ -463,27 +499,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC3E447-3B6A-9040-A6A4-DC20E2513405}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="10.83203125" style="1"/>
+    <col min="3" max="3" width="10.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1"/>
     <col min="7" max="7" width="18.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="11" width="10.83203125" style="1"/>
     <col min="12" max="12" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" style="1"/>
+    <col min="13" max="13" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="20.5" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="18.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11.5" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -524,7 +563,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -569,8 +608,12 @@
         <f>M2/N2</f>
         <v>2.6639555057854154</v>
       </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="P2" s="1">
+        <f xml:space="preserve"> 3* O2</f>
+        <v>7.9918665173562466</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -616,7 +659,7 @@
         <v>2.7043551271731201</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -662,7 +705,7 @@
         <v>2.8183657857060198</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -708,7 +751,7 @@
         <v>0.9620020738120264</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -754,7 +797,7 @@
         <v>2.4633967625718953</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
@@ -777,7 +820,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -788,8 +831,8 @@
         <v>-12.91</v>
       </c>
       <c r="D9" s="1">
-        <f>D2 + 7.98</f>
-        <v>16.585230967266366</v>
+        <f>D2 + O3 * 3</f>
+        <v>16.718296348785728</v>
       </c>
       <c r="E9" s="1">
         <f>SQRT((POWER(B9,2))+(POWER(C9,2)))</f>
@@ -805,18 +848,18 @@
       </c>
       <c r="J9" s="1">
         <f>ACOS(B9/D9)*180/PI()</f>
-        <v>51.148423489676951</v>
+        <v>51.514818171535559</v>
       </c>
       <c r="K9" s="1">
         <f>180 - ACOS(C9 /D9)*180/PI()</f>
-        <v>38.885377194155353</v>
+        <v>39.447430319968191</v>
       </c>
       <c r="L9" s="1">
         <f xml:space="preserve"> J9 + K9</f>
-        <v>90.033800683832311</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
+        <v>90.962248491503743</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B10" s="1">
         <v>10.467000000000001</v>
       </c>
@@ -824,8 +867,8 @@
         <v>-12.442</v>
       </c>
       <c r="D10" s="1">
-        <f>D3 + 7.98</f>
-        <v>16.259721976008613</v>
+        <f>D3 + O2 * 3</f>
+        <v>16.27158849336486</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" ref="E10:E13" si="2">SQRT((POWER(B10,2))+(POWER(C10,2)))</f>
@@ -841,18 +884,18 @@
       </c>
       <c r="J10" s="1">
         <f t="shared" ref="J10:J13" si="5">ACOS(B10/D10)*180/PI()</f>
-        <v>49.928883307189778</v>
+        <v>49.964024135951192</v>
       </c>
       <c r="K10" s="1">
         <f t="shared" ref="K10:K13" si="6">180 - ACOS(C10 /D10)*180/PI()</f>
-        <v>40.074879336209705</v>
+        <v>40.124518737124845</v>
       </c>
       <c r="L10" s="1">
         <f t="shared" ref="L10:L13" si="7" xml:space="preserve"> J10 + K10</f>
-        <v>90.003762643399483</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
+        <v>90.088542873076037</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B11" s="1">
         <v>16.66</v>
       </c>
@@ -888,7 +931,7 @@
         <v>89.915642912055006</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
         <v>7.1064226882000003</v>
       </c>
@@ -923,7 +966,7 @@
         <v>90.351820358332915</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
         <v>10.102544120999999</v>
       </c>
@@ -957,6 +1000,346 @@
       <c r="L13" s="1">
         <f t="shared" si="7"/>
         <v>90.000000008151403</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B18" s="2">
+        <v>8.4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>-9.6999999999999993</v>
+      </c>
+      <c r="D18" s="1">
+        <f>SQRT((POWER(B18,2))+(POWER(C18,2)))</f>
+        <v>12.83160161476345</v>
+      </c>
+      <c r="G18" s="2">
+        <v>51.132222499999997</v>
+      </c>
+      <c r="H18" s="2">
+        <v>38.867777500000003</v>
+      </c>
+      <c r="J18" s="1">
+        <f>ACOS(B18/D18)*180/PI()</f>
+        <v>49.108112177135865</v>
+      </c>
+      <c r="K18" s="1">
+        <f>180 - ACOS(C18/D18)*180/PI()</f>
+        <v>40.891887822864135</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B19" s="2">
+        <v>8.33</v>
+      </c>
+      <c r="C19" s="2">
+        <v>-9.3360000000000003</v>
+      </c>
+      <c r="D19" s="1">
+        <f>SQRT((POWER(B19,2))+(POWER(C19,2)))</f>
+        <v>12.511986093342657</v>
+      </c>
+      <c r="G19" s="2">
+        <v>49.928622910000001</v>
+      </c>
+      <c r="H19" s="2">
+        <v>40.071377099999999</v>
+      </c>
+      <c r="J19" s="1">
+        <f>ACOS(B19/D19)*180/PI()</f>
+        <v>48.259219444860257</v>
+      </c>
+      <c r="K19" s="1">
+        <f>180 - ACOS(C19/D19)*180/PI()</f>
+        <v>41.740780555139736</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B20" s="2">
+        <v>9.66</v>
+      </c>
+      <c r="C20" s="2">
+        <v>-11.2</v>
+      </c>
+      <c r="D20" s="1">
+        <f>SQRT((POWER(B20,2))+(POWER(C20,2)))</f>
+        <v>14.790388771090502</v>
+      </c>
+      <c r="G20" s="2">
+        <v>50.91666472</v>
+      </c>
+      <c r="H20" s="2">
+        <v>39.083335300000002</v>
+      </c>
+      <c r="J20" s="1">
+        <f>ACOS(B20/D20)*180/PI()</f>
+        <v>49.222230206142683</v>
+      </c>
+      <c r="K20" s="1">
+        <f>180 - ACOS(C20/D20)*180/PI()</f>
+        <v>40.777769793857289</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B21" s="2">
+        <v>9.33</v>
+      </c>
+      <c r="C21" s="2">
+        <v>-11.51</v>
+      </c>
+      <c r="D21" s="1">
+        <f>SQRT((POWER(B21,2))+(POWER(C21,2)))</f>
+        <v>14.816511060300263</v>
+      </c>
+      <c r="G21" s="2">
+        <v>53.356993750000001</v>
+      </c>
+      <c r="H21" s="2">
+        <v>36.643006200000002</v>
+      </c>
+      <c r="J21" s="1">
+        <f>ACOS(B21/D21)*180/PI()</f>
+        <v>50.971793476032751</v>
+      </c>
+      <c r="K21" s="1">
+        <f>180 - ACOS(C21/D21)*180/PI()</f>
+        <v>39.028206523967242</v>
+      </c>
+      <c r="O21" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B22" s="2">
+        <v>9.98</v>
+      </c>
+      <c r="C22" s="2">
+        <v>-12.65</v>
+      </c>
+      <c r="D22" s="1">
+        <f>SQRT((POWER(B22,2))+(POWER(C22,2)))</f>
+        <v>16.11281787894346</v>
+      </c>
+      <c r="G22" s="2">
+        <v>54.121180070000001</v>
+      </c>
+      <c r="H22" s="2">
+        <v>35.878819900000003</v>
+      </c>
+      <c r="J22" s="1">
+        <f>ACOS(B22/D22)*180/PI()</f>
+        <v>51.728932951997166</v>
+      </c>
+      <c r="K22" s="1">
+        <f>180 - ACOS(C22/D22)*180/PI()</f>
+        <v>38.271067048002806</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A25" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B26" s="1">
+        <v>7.55</v>
+      </c>
+      <c r="C26" s="1">
+        <v>-9.3800000000000008</v>
+      </c>
+      <c r="D26" s="1">
+        <f>SQRT((POWER(B26,2))+(POWER(C26,2)))</f>
+        <v>12.041050618612978</v>
+      </c>
+      <c r="E26" s="1">
+        <v>12</v>
+      </c>
+      <c r="G26" s="1">
+        <f>ACOS(B26/12.04159458)*180/PI()</f>
+        <v>51.171354255815359</v>
+      </c>
+      <c r="H26" s="1">
+        <f>180 - ACOS(C26/12.04159458)*180/PI()</f>
+        <v>38.83394450104629</v>
+      </c>
+      <c r="I26" s="1">
+        <f xml:space="preserve"> G26 + H26</f>
+        <v>90.005298756861649</v>
+      </c>
+      <c r="J26" s="1">
+        <f>ACOS(B26/D26)*180/PI()</f>
+        <v>51.169270991081412</v>
+      </c>
+      <c r="K26" s="1">
+        <f>180 - ACOS(C26/D26)*180/PI()</f>
+        <v>38.830729008918553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B27" s="1">
+        <v>7.64</v>
+      </c>
+      <c r="C27" s="1">
+        <v>-9.08</v>
+      </c>
+      <c r="D27" s="1">
+        <f>SQRT((POWER(B27,2))+(POWER(C27,2)))</f>
+        <v>11.866591760063207</v>
+      </c>
+      <c r="E27" s="1">
+        <v>12</v>
+      </c>
+      <c r="G27" s="1">
+        <f>ACOS(B27/11.86307296)*180/PI()</f>
+        <v>49.908116965276271</v>
+      </c>
+      <c r="H27" s="1">
+        <f>180 - ACOS(C27/11.86307296)*180/PI()</f>
+        <v>40.057379386721209</v>
+      </c>
+      <c r="I27" s="1">
+        <f t="shared" ref="I27:I30" si="8" xml:space="preserve"> G27 + H27</f>
+        <v>89.965496351997473</v>
+      </c>
+      <c r="J27" s="1">
+        <f>ACOS(B27/D27)*180/PI()</f>
+        <v>49.922418187135989</v>
+      </c>
+      <c r="K27" s="1">
+        <f>180 - ACOS(C27/D27)*180/PI()</f>
+        <v>40.077581812863997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B28" s="1">
+        <v>8.9700000000000006</v>
+      </c>
+      <c r="C28" s="1">
+        <v>-11.02</v>
+      </c>
+      <c r="D28" s="1">
+        <f>SQRT((POWER(B28,2))+(POWER(C28,2)))</f>
+        <v>14.209197725417154</v>
+      </c>
+      <c r="E28" s="1">
+        <v>14</v>
+      </c>
+      <c r="G28" s="1">
+        <f>ACOS(B28/14.2126704)*180/PI()</f>
+        <v>50.866680582364388</v>
+      </c>
+      <c r="H28" s="1">
+        <f>180 - ACOS(C28/14.2126704)*180/PI()</f>
+        <v>39.161909404704829</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" si="8"/>
+        <v>90.028589987069211</v>
+      </c>
+      <c r="J28" s="1">
+        <f>ACOS(B28/D28)*180/PI()</f>
+        <v>50.855286306268873</v>
+      </c>
+      <c r="K28" s="1">
+        <f>180 - ACOS(C28/D28)*180/PI()</f>
+        <v>39.144713693731148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B29" s="1">
+        <v>7.61</v>
+      </c>
+      <c r="C29" s="1">
+        <v>-10.220000000000001</v>
+      </c>
+      <c r="D29" s="1">
+        <f>SQRT((POWER(B29,2))+(POWER(C29,2)))</f>
+        <v>12.742075969009132</v>
+      </c>
+      <c r="E29" s="1">
+        <v>12.5</v>
+      </c>
+      <c r="G29" s="1">
+        <f>ACOS(B29/12.74754878)*180/PI()</f>
+        <v>53.346266543602297</v>
+      </c>
+      <c r="H29" s="1">
+        <f>180 - ACOS(C29/12.74754878)*180/PI()</f>
+        <v>36.705069773775904</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="8"/>
+        <v>90.051336317378201</v>
+      </c>
+      <c r="J29" s="1">
+        <f>ACOS(B29/D29)*180/PI()</f>
+        <v>53.327952321058113</v>
+      </c>
+      <c r="K29" s="1">
+        <f>180 - ACOS(C29/D29)*180/PI()</f>
+        <v>36.67204767894188</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="B30" s="1">
+        <v>9.17</v>
+      </c>
+      <c r="C30" s="1">
+        <v>-12.65</v>
+      </c>
+      <c r="D30" s="1">
+        <f>SQRT((POWER(B30,2))+(POWER(C30,2)))</f>
+        <v>15.624064772011156</v>
+      </c>
+      <c r="E30" s="1">
+        <v>15</v>
+      </c>
+      <c r="G30" s="1">
+        <f>ACOS(B30/15.62049935)*180/PI()</f>
+        <v>54.052118563647404</v>
+      </c>
+      <c r="H30" s="1">
+        <f>180 - ACOS(C30/15.62049935)*180/PI()</f>
+        <v>35.920355779523675</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="8"/>
+        <v>89.972474343171086</v>
+      </c>
+      <c r="J30" s="1">
+        <f>ACOS(B30/D30)*180/PI()</f>
+        <v>54.061599331669292</v>
+      </c>
+      <c r="K30" s="1">
+        <f>180 - ACOS(C30/D30)*180/PI()</f>
+        <v>35.938400668330701</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the excel file
</commit_message>
<xml_diff>
--- a/Sounding_calculation.xlsx
+++ b/Sounding_calculation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/FireFlux_med/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6B383A-D337-154E-9C92-E97D98C8343D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36961D3D-5CA4-4C43-861C-1B4BF7E3246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{BE37ABCF-635B-BF46-BE11-3CD29516FACD}"/>
+    <workbookView xWindow="72960" yWindow="-7220" windowWidth="38400" windowHeight="21600" xr2:uid="{BE37ABCF-635B-BF46-BE11-3CD29516FACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="24">
   <si>
     <t>Original input_Sounding</t>
   </si>
@@ -130,7 +130,10 @@
     <t>thoughts</t>
   </si>
   <si>
-    <t>f</t>
+    <t>Averages</t>
+  </si>
+  <si>
+    <t>5.46m</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CC3E447-3B6A-9040-A6A4-DC20E2513405}">
-  <dimension ref="A1:P30"/>
+  <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -930,6 +933,14 @@
         <f t="shared" si="7"/>
         <v>89.915642912055006</v>
       </c>
+      <c r="N11" s="1">
+        <f>D4 - E4</f>
+        <v>4.7919018622701381</v>
+      </c>
+      <c r="O11" s="1">
+        <f t="shared" ref="O11:O12" si="8" xml:space="preserve"> N11 * O4</f>
+        <v>13.505332257083117</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B12" s="1">
@@ -965,6 +976,14 @@
         <f t="shared" si="7"/>
         <v>90.351820358332915</v>
       </c>
+      <c r="N12" s="1">
+        <f>D5 - E5</f>
+        <v>1.5585691601491796</v>
+      </c>
+      <c r="O12" s="1">
+        <f t="shared" si="8"/>
+        <v>1.499346764242979</v>
+      </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B13" s="1">
@@ -1001,8 +1020,16 @@
         <f t="shared" si="7"/>
         <v>90.000000008151403</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="N13" s="1">
+        <f>D6 - E6</f>
+        <v>2.0703676940530027</v>
+      </c>
+      <c r="O13" s="1">
+        <f xml:space="preserve"> N13 * O6</f>
+        <v>5.100137074863607</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>20</v>
       </c>
@@ -1020,7 +1047,7 @@
       </c>
       <c r="H17" s="2"/>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B18" s="2">
         <v>8.4</v>
       </c>
@@ -1046,7 +1073,7 @@
         <v>40.891887822864135</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B19" s="2">
         <v>8.33</v>
       </c>
@@ -1072,7 +1099,7 @@
         <v>41.740780555139736</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B20" s="2">
         <v>9.66</v>
       </c>
@@ -1098,7 +1125,7 @@
         <v>40.777769793857289</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B21" s="2">
         <v>9.33</v>
       </c>
@@ -1123,11 +1150,8 @@
         <f>180 - ACOS(C21/D21)*180/PI()</f>
         <v>39.028206523967242</v>
       </c>
-      <c r="O21" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B22" s="2">
         <v>9.98</v>
       </c>
@@ -1153,7 +1177,7 @@
         <v>38.271067048002806</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>21</v>
       </c>
@@ -1167,7 +1191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B26" s="1">
         <v>7.55</v>
       </c>
@@ -1202,7 +1226,7 @@
         <v>38.830729008918553</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B27" s="1">
         <v>7.64</v>
       </c>
@@ -1225,7 +1249,7 @@
         <v>40.057379386721209</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" ref="I27:I30" si="8" xml:space="preserve"> G27 + H27</f>
+        <f t="shared" ref="I27:I30" si="9" xml:space="preserve"> G27 + H27</f>
         <v>89.965496351997473</v>
       </c>
       <c r="J27" s="1">
@@ -1237,7 +1261,7 @@
         <v>40.077581812863997</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B28" s="1">
         <v>8.9700000000000006</v>
       </c>
@@ -1260,7 +1284,7 @@
         <v>39.161909404704829</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>90.028589987069211</v>
       </c>
       <c r="J28" s="1">
@@ -1272,7 +1296,7 @@
         <v>39.144713693731148</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B29" s="1">
         <v>7.61</v>
       </c>
@@ -1295,7 +1319,7 @@
         <v>36.705069773775904</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>90.051336317378201</v>
       </c>
       <c r="J29" s="1">
@@ -1307,7 +1331,7 @@
         <v>36.67204767894188</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="B30" s="1">
         <v>9.17</v>
       </c>
@@ -1330,7 +1354,7 @@
         <v>35.920355779523675</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>89.972474343171086</v>
       </c>
       <c r="J30" s="1">
@@ -1340,6 +1364,112 @@
       <c r="K30" s="1">
         <f>180 - ACOS(C30/D30)*180/PI()</f>
         <v>35.938400668330701</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="1">
+        <f>AVERAGE(D2:D4) + 3</f>
+        <v>12.149611601848372</v>
+      </c>
+      <c r="D35" s="1">
+        <v>7.702</v>
+      </c>
+      <c r="E35" s="1">
+        <v>-9.3960000000000008</v>
+      </c>
+      <c r="F35" s="1">
+        <v>12.1496116</v>
+      </c>
+      <c r="G35" s="1">
+        <f>SQRT((POWER(D35,2)+POWER(E35,2)))</f>
+        <v>12.149305329935535</v>
+      </c>
+      <c r="H35" s="1">
+        <f>AVERAGE(G18:G20)</f>
+        <v>50.659170043333326</v>
+      </c>
+      <c r="I35" s="1">
+        <f>AVERAGE(H18:H20)</f>
+        <v>39.340829966666668</v>
+      </c>
+      <c r="L35" s="1">
+        <v>289.07</v>
+      </c>
+      <c r="M35" s="1">
+        <f>AVERAGE(L35:L37)</f>
+        <v>288.11666666666662</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B36" s="1">
+        <f>D5 + 3</f>
+        <v>13.606083160149179</v>
+      </c>
+      <c r="D36" s="1">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="E36" s="1">
+        <v>-10.917</v>
+      </c>
+      <c r="F36" s="1">
+        <v>13.6060832</v>
+      </c>
+      <c r="G36" s="1">
+        <f>SQRT((POWER(D36,2)+POWER(E36,2)))</f>
+        <v>13.605707956589395</v>
+      </c>
+      <c r="H36" s="2">
+        <v>53.356993750000001</v>
+      </c>
+      <c r="I36" s="2">
+        <v>36.643006200000002</v>
+      </c>
+      <c r="L36" s="1">
+        <v>288.23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B37" s="1">
+        <f>D6 + O13</f>
+        <v>17.009918768916609</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9.9700000000000006</v>
+      </c>
+      <c r="E37" s="1">
+        <v>-13.78</v>
+      </c>
+      <c r="G37" s="1">
+        <f>SQRT((POWER(D37,2)+POWER(E37,2)))</f>
+        <v>17.008506695180504</v>
+      </c>
+      <c r="H37" s="2">
+        <v>54.121180070000001</v>
+      </c>
+      <c r="I37" s="2">
+        <v>35.878819900000003</v>
+      </c>
+      <c r="L37" s="1">
+        <v>287.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adjusting the new sounding and creating plots to see how much I need to increase the upper level winds
</commit_message>
<xml_diff>
--- a/Sounding_calculation.xlsx
+++ b/Sounding_calculation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_files/FireFlux_med/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeremybenik/Research_Files/FireFlux_med/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36961D3D-5CA4-4C43-861C-1B4BF7E3246F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52F0A97F-825A-2648-A3E8-581F9D231985}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="72960" yWindow="-7220" windowWidth="38400" windowHeight="21600" xr2:uid="{BE37ABCF-635B-BF46-BE11-3CD29516FACD}"/>
+    <workbookView xWindow="0" yWindow="640" windowWidth="34560" windowHeight="21700" xr2:uid="{BE37ABCF-635B-BF46-BE11-3CD29516FACD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -505,7 +505,7 @@
   <dimension ref="A1:P37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+      <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1458,6 +1458,10 @@
       <c r="E37" s="1">
         <v>-13.78</v>
       </c>
+      <c r="F37" s="1">
+        <f>SQRT((POWER(D37,2))+(POWER(E37,2)))</f>
+        <v>17.008506695180504</v>
+      </c>
       <c r="G37" s="1">
         <f>SQRT((POWER(D37,2)+POWER(E37,2)))</f>
         <v>17.008506695180504</v>

</xml_diff>